<commit_message>
add test for nosql database
</commit_message>
<xml_diff>
--- a/hammer-colombo/nosql-examaples-set/test.xlsx
+++ b/hammer-colombo/nosql-examaples-set/test.xlsx
@@ -1,25 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MauroRepository/My_Repository/CRISP_Progetti/Hammer_Project/git/hammer-colombo/nosql-examaples-set/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E65DC05-35C3-EB47-A1DA-3487573317ED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="460" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="5" r:id="rId1"/>
     <sheet name="testbed" sheetId="7" r:id="rId2"/>
     <sheet name="baseline" sheetId="6" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="47">
   <si>
     <t>th_krm</t>
   </si>
@@ -159,12 +166,24 @@
   </si>
   <si>
     <t xml:space="preserve">th_query </t>
+  </si>
+  <si>
+    <t>5_nosql</t>
+  </si>
+  <si>
+    <t>6_nosql</t>
+  </si>
+  <si>
+    <t>7_nosql</t>
+  </si>
+  <si>
+    <t>8_nosql</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -347,7 +366,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -432,47 +451,6 @@
       <left style="medium">
         <color auto="1"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -509,19 +487,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -758,7 +723,24 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color auto="1"/>
       </right>
@@ -771,118 +753,127 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
       <top style="thin">
         <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -895,7 +886,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -903,25 +894,18 @@
     </xf>
     <xf numFmtId="10" fontId="6" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="6" fillId="7" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="6" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="10" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="10" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="10" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="10" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -930,156 +914,159 @@
     <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="6" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="10" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="10" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="10" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="10" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="10" fillId="10" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="10" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="0" borderId="41" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="2" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="10" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="10" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="10" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="10" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Collegamento ipertestuale" xfId="2" builtinId="8"/>
@@ -1364,11 +1351,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:S8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:S12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1380,170 +1367,170 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="38" t="s">
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
     </row>
     <row r="2" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="43" t="s">
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="40" t="s">
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="42"/>
-      <c r="P2" s="43" t="s">
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="44"/>
-      <c r="S2" s="45"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="58"/>
+      <c r="S2" s="59"/>
     </row>
     <row r="3" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="84" t="s">
+      <c r="D3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="85" t="s">
+      <c r="E3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="95" t="s">
+      <c r="F3" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="85" t="s">
+      <c r="G3" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="84" t="s">
+      <c r="H3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="85" t="s">
+      <c r="I3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="95" t="s">
+      <c r="J3" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="85" t="s">
+      <c r="K3" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="84" t="s">
+      <c r="L3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="85" t="s">
+      <c r="M3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="95" t="s">
+      <c r="N3" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="85" t="s">
+      <c r="O3" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="84" t="s">
+      <c r="P3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="85" t="s">
+      <c r="Q3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="95" t="s">
+      <c r="R3" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="85" t="s">
+      <c r="S3" s="30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="86">
-        <v>1</v>
-      </c>
-      <c r="E4" s="87">
-        <v>1</v>
-      </c>
-      <c r="F4" s="96">
-        <v>1</v>
-      </c>
-      <c r="G4" s="87">
-        <v>1</v>
-      </c>
-      <c r="H4" s="86">
-        <v>1</v>
-      </c>
-      <c r="I4" s="87">
+      <c r="D4" s="31">
+        <v>1</v>
+      </c>
+      <c r="E4" s="32">
+        <v>1</v>
+      </c>
+      <c r="F4" s="38">
+        <v>1</v>
+      </c>
+      <c r="G4" s="33">
+        <v>1</v>
+      </c>
+      <c r="H4" s="31">
+        <v>1</v>
+      </c>
+      <c r="I4" s="32">
         <v>0.33329999999999999</v>
       </c>
-      <c r="J4" s="96">
-        <v>1</v>
-      </c>
-      <c r="K4" s="88">
+      <c r="J4" s="38">
+        <v>1</v>
+      </c>
+      <c r="K4" s="33">
         <v>0.33329999999999999</v>
       </c>
-      <c r="L4" s="92">
-        <v>1</v>
-      </c>
-      <c r="M4" s="87">
-        <v>1</v>
-      </c>
-      <c r="N4" s="96">
-        <v>1</v>
-      </c>
-      <c r="O4" s="88">
-        <v>1</v>
-      </c>
-      <c r="P4" s="86">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="87">
-        <v>1</v>
-      </c>
-      <c r="R4" s="96">
-        <v>1</v>
-      </c>
-      <c r="S4" s="88">
+      <c r="L4" s="31">
+        <v>1</v>
+      </c>
+      <c r="M4" s="32">
+        <v>1</v>
+      </c>
+      <c r="N4" s="38">
+        <v>1</v>
+      </c>
+      <c r="O4" s="33">
+        <v>1</v>
+      </c>
+      <c r="P4" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="32">
+        <v>1</v>
+      </c>
+      <c r="R4" s="38">
+        <v>1</v>
+      </c>
+      <c r="S4" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="24" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="3">
@@ -1552,10 +1539,10 @@
       <c r="E5" s="4">
         <v>1</v>
       </c>
-      <c r="F5" s="97">
-        <v>1</v>
-      </c>
-      <c r="G5" s="4">
+      <c r="F5" s="39">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5">
         <v>1</v>
       </c>
       <c r="H5" s="3">
@@ -1564,22 +1551,22 @@
       <c r="I5" s="4">
         <v>1</v>
       </c>
-      <c r="J5" s="97">
-        <v>1</v>
-      </c>
-      <c r="K5" s="6">
-        <v>1</v>
-      </c>
-      <c r="L5" s="11">
+      <c r="J5" s="39">
+        <v>1</v>
+      </c>
+      <c r="K5" s="5">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3">
         <v>1</v>
       </c>
       <c r="M5" s="4">
         <v>1</v>
       </c>
-      <c r="N5" s="97">
-        <v>1</v>
-      </c>
-      <c r="O5" s="4">
+      <c r="N5" s="39">
+        <v>1</v>
+      </c>
+      <c r="O5" s="5">
         <v>1</v>
       </c>
       <c r="P5" s="3">
@@ -1588,18 +1575,18 @@
       <c r="Q5" s="4">
         <v>1</v>
       </c>
-      <c r="R5" s="97">
-        <v>1</v>
-      </c>
-      <c r="S5" s="6">
+      <c r="R5" s="39">
+        <v>1</v>
+      </c>
+      <c r="S5" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="24" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="3">
@@ -1608,7 +1595,7 @@
       <c r="E6" s="4">
         <v>1</v>
       </c>
-      <c r="F6" s="97">
+      <c r="F6" s="39">
         <v>1</v>
       </c>
       <c r="G6" s="5">
@@ -1620,157 +1607,381 @@
       <c r="I6" s="4">
         <v>0.33329999999999999</v>
       </c>
-      <c r="J6" s="97">
+      <c r="J6" s="39">
         <v>0.33329999999999999</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="5">
         <v>0.33329999999999999</v>
       </c>
-      <c r="L6" s="83">
+      <c r="L6" s="46">
         <v>0</v>
       </c>
-      <c r="M6" s="82">
+      <c r="M6" s="28">
         <v>0</v>
       </c>
-      <c r="N6" s="97">
-        <v>1</v>
-      </c>
-      <c r="O6" s="6">
-        <v>1</v>
-      </c>
-      <c r="P6" s="82">
+      <c r="N6" s="39">
+        <v>1</v>
+      </c>
+      <c r="O6" s="5">
+        <v>1</v>
+      </c>
+      <c r="P6" s="46">
         <v>0</v>
       </c>
-      <c r="Q6" s="82">
+      <c r="Q6" s="28">
         <v>0</v>
       </c>
-      <c r="R6" s="97">
-        <v>1</v>
-      </c>
-      <c r="S6" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+      <c r="R6" s="39">
+        <v>1</v>
+      </c>
+      <c r="S6" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="89">
-        <v>1</v>
-      </c>
-      <c r="E7" s="90">
-        <v>1</v>
-      </c>
-      <c r="F7" s="98">
-        <v>1</v>
-      </c>
-      <c r="G7" s="93">
-        <v>1</v>
-      </c>
-      <c r="H7" s="89">
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="39">
+        <v>1</v>
+      </c>
+      <c r="G7" s="5">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3">
         <v>0.33329999999999999</v>
       </c>
-      <c r="I7" s="90">
+      <c r="I7" s="4">
         <v>0.33329999999999999</v>
       </c>
-      <c r="J7" s="98">
+      <c r="J7" s="39">
         <v>0.33329999999999999</v>
       </c>
-      <c r="K7" s="91">
+      <c r="K7" s="5">
         <v>0.33329999999999999</v>
       </c>
-      <c r="L7" s="94">
+      <c r="L7" s="46">
         <v>0</v>
       </c>
-      <c r="M7" s="94">
+      <c r="M7" s="28">
         <v>0</v>
       </c>
-      <c r="N7" s="98">
-        <v>1</v>
-      </c>
-      <c r="O7" s="91">
-        <v>1</v>
-      </c>
-      <c r="P7" s="94">
+      <c r="N7" s="39">
+        <v>1</v>
+      </c>
+      <c r="O7" s="5">
+        <v>1</v>
+      </c>
+      <c r="P7" s="46">
         <v>0</v>
       </c>
-      <c r="Q7" s="94">
+      <c r="Q7" s="28">
         <v>0</v>
       </c>
-      <c r="R7" s="98">
+      <c r="R7" s="39">
         <v>0.70369999999999999</v>
       </c>
-      <c r="S7" s="91">
+      <c r="S7" s="5">
         <v>0.70369999999999999</v>
       </c>
     </row>
-    <row r="8" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="12">
-        <f t="shared" ref="D8:S8" si="0">AVERAGE(D4:D7)</f>
-        <v>1</v>
-      </c>
-      <c r="E8" s="13">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="39">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="J8" s="39">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="K8" s="5">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="L8" s="3">
+        <v>1</v>
+      </c>
+      <c r="M8" s="4">
+        <v>1</v>
+      </c>
+      <c r="N8" s="39">
+        <v>1</v>
+      </c>
+      <c r="O8" s="5">
+        <v>1</v>
+      </c>
+      <c r="P8" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>1</v>
+      </c>
+      <c r="R8" s="39">
+        <v>1</v>
+      </c>
+      <c r="S8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B9" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
+      <c r="F9" s="39">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="4">
+        <v>1</v>
+      </c>
+      <c r="J9" s="39">
+        <v>1</v>
+      </c>
+      <c r="K9" s="5">
+        <v>1</v>
+      </c>
+      <c r="L9" s="46">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4">
+        <v>1</v>
+      </c>
+      <c r="N9" s="39">
+        <v>1</v>
+      </c>
+      <c r="O9" s="5">
+        <v>1</v>
+      </c>
+      <c r="P9" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>0.27779999999999999</v>
+      </c>
+      <c r="R9" s="39">
+        <v>0.27779999999999999</v>
+      </c>
+      <c r="S9" s="5">
+        <v>0.27779999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" s="39">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+      <c r="I10" s="4">
+        <v>1</v>
+      </c>
+      <c r="J10" s="39">
+        <v>1</v>
+      </c>
+      <c r="K10" s="5">
+        <v>1</v>
+      </c>
+      <c r="L10" s="46">
+        <v>0</v>
+      </c>
+      <c r="M10" s="4">
+        <v>1</v>
+      </c>
+      <c r="N10" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="O10" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="P10" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>1</v>
+      </c>
+      <c r="R10" s="39">
+        <v>1</v>
+      </c>
+      <c r="S10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="34">
+        <v>1</v>
+      </c>
+      <c r="E11" s="35">
+        <v>1</v>
+      </c>
+      <c r="F11" s="40">
+        <v>1</v>
+      </c>
+      <c r="G11" s="36">
+        <v>1</v>
+      </c>
+      <c r="H11" s="34">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="I11" s="35">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="J11" s="40">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="K11" s="36">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="L11" s="34">
+        <v>1</v>
+      </c>
+      <c r="M11" s="35">
+        <v>1</v>
+      </c>
+      <c r="N11" s="40">
+        <v>1</v>
+      </c>
+      <c r="O11" s="36">
+        <v>1</v>
+      </c>
+      <c r="P11" s="34">
+        <v>4.4400000000000002E-2</v>
+      </c>
+      <c r="Q11" s="35">
+        <v>4.4400000000000002E-2</v>
+      </c>
+      <c r="R11" s="40">
+        <v>4.5499999999999999E-2</v>
+      </c>
+      <c r="S11" s="36">
+        <v>4.5499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="41">
+        <f>AVERAGE(D4:D11)</f>
+        <v>1</v>
+      </c>
+      <c r="E12" s="42">
+        <f t="shared" ref="E12:S12" si="0">AVERAGE(E4:E11)</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="43">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F8" s="99">
+      <c r="G12" s="44">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G8" s="33">
+      <c r="H12" s="41">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H8" s="12">
+        <v>0.74998750000000003</v>
+      </c>
+      <c r="I12" s="42">
         <f t="shared" si="0"/>
-        <v>0.83332499999999998</v>
-      </c>
-      <c r="I8" s="13">
+        <v>0.58331250000000001</v>
+      </c>
+      <c r="J12" s="43">
         <f t="shared" si="0"/>
-        <v>0.49997499999999995</v>
-      </c>
-      <c r="J8" s="99">
+        <v>0.66665000000000008</v>
+      </c>
+      <c r="K12" s="45">
         <f t="shared" si="0"/>
-        <v>0.66664999999999996</v>
-      </c>
-      <c r="K8" s="14">
-        <f t="shared" si="0"/>
-        <v>0.49997499999999995</v>
-      </c>
-      <c r="L8" s="12">
+        <v>0.58331250000000001</v>
+      </c>
+      <c r="L12" s="41">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M12" s="42">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="N8" s="99">
+        <v>0.75</v>
+      </c>
+      <c r="N12" s="43">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="O8" s="14">
+        <v>0.9375</v>
+      </c>
+      <c r="O12" s="45">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="P8" s="12">
+        <v>0.9375</v>
+      </c>
+      <c r="P12" s="41">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="Q8" s="13">
+        <v>0.38055</v>
+      </c>
+      <c r="Q12" s="42">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="R8" s="99">
+        <v>0.54027500000000006</v>
+      </c>
+      <c r="R12" s="43">
         <f t="shared" si="0"/>
-        <v>0.925925</v>
-      </c>
-      <c r="S8" s="14">
+        <v>0.75337499999999991</v>
+      </c>
+      <c r="S12" s="45">
         <f t="shared" si="0"/>
-        <v>0.925925</v>
+        <v>0.75337499999999991</v>
       </c>
     </row>
   </sheetData>
@@ -1787,7 +1998,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:U11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1797,287 +2008,297 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="3" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="25"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="18"/>
     </row>
     <row r="4" spans="2:21" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="65" t="s">
+      <c r="C4" s="60"/>
+      <c r="D4" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="65" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="65" t="s">
+      <c r="E4" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="72" t="s">
+      <c r="G4" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="65" t="s">
+      <c r="H4" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="54"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="49"/>
-      <c r="O4" s="50"/>
-      <c r="P4" s="66" t="s">
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="80"/>
+      <c r="M4" s="74"/>
+      <c r="N4" s="75"/>
+      <c r="O4" s="76"/>
+      <c r="P4" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="68"/>
-      <c r="T4" s="47"/>
-      <c r="U4" s="46"/>
+      <c r="Q4" s="63"/>
+      <c r="R4" s="63"/>
+      <c r="S4" s="64"/>
+      <c r="T4" s="73"/>
+      <c r="U4" s="68"/>
     </row>
     <row r="5" spans="2:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="72"/>
-      <c r="J5" s="65"/>
-      <c r="K5" s="65"/>
-      <c r="L5" s="54"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="53"/>
-      <c r="P5" s="69" t="s">
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="69"/>
+      <c r="J5" s="61"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="77"/>
+      <c r="N5" s="78"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="Q5" s="70"/>
-      <c r="R5" s="70"/>
-      <c r="S5" s="71"/>
-      <c r="T5" s="47"/>
-      <c r="U5" s="46"/>
+      <c r="Q5" s="66"/>
+      <c r="R5" s="66"/>
+      <c r="S5" s="67"/>
+      <c r="T5" s="73"/>
+      <c r="U5" s="68"/>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="26" t="s">
+      <c r="C6" s="18"/>
+      <c r="D6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="18">
         <v>3</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H6" s="18">
         <v>10</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="61" t="s">
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="N6" s="62"/>
-      <c r="O6" s="63"/>
-      <c r="P6" s="61">
+      <c r="N6" s="71"/>
+      <c r="O6" s="72"/>
+      <c r="P6" s="70">
         <v>3</v>
       </c>
-      <c r="Q6" s="62"/>
-      <c r="R6" s="62"/>
-      <c r="S6" s="63"/>
-      <c r="T6" s="25"/>
-      <c r="U6" s="25"/>
+      <c r="Q6" s="71"/>
+      <c r="R6" s="71"/>
+      <c r="S6" s="72"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="18"/>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="26" t="s">
+      <c r="C7" s="18"/>
+      <c r="D7" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="18">
         <v>3</v>
       </c>
-      <c r="H7" s="25">
+      <c r="H7" s="18">
         <v>10</v>
       </c>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="61" t="s">
+      <c r="I7" s="68"/>
+      <c r="J7" s="68"/>
+      <c r="K7" s="68"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="N7" s="62"/>
-      <c r="O7" s="63"/>
-      <c r="P7" s="61">
+      <c r="N7" s="71"/>
+      <c r="O7" s="72"/>
+      <c r="P7" s="70">
         <v>32</v>
       </c>
-      <c r="Q7" s="62"/>
-      <c r="R7" s="62"/>
-      <c r="S7" s="63"/>
-      <c r="T7" s="25"/>
-      <c r="U7" s="25"/>
+      <c r="Q7" s="71"/>
+      <c r="R7" s="71"/>
+      <c r="S7" s="72"/>
+      <c r="T7" s="18"/>
+      <c r="U7" s="18"/>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="29" t="s">
+      <c r="C8" s="21"/>
+      <c r="D8" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="E8" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="21">
         <v>3</v>
       </c>
-      <c r="H8" s="28">
+      <c r="H8" s="21">
         <v>10</v>
       </c>
-      <c r="I8" s="28" t="s">
+      <c r="I8" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="61" t="s">
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="N8" s="62"/>
-      <c r="O8" s="63"/>
-      <c r="P8" s="61">
+      <c r="N8" s="71"/>
+      <c r="O8" s="72"/>
+      <c r="P8" s="70">
         <v>3000</v>
       </c>
-      <c r="Q8" s="62"/>
-      <c r="R8" s="62"/>
-      <c r="S8" s="63"/>
-      <c r="T8" s="25"/>
-      <c r="U8" s="25"/>
+      <c r="Q8" s="71"/>
+      <c r="R8" s="71"/>
+      <c r="S8" s="72"/>
+      <c r="T8" s="18"/>
+      <c r="U8" s="18"/>
     </row>
     <row r="9" spans="2:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="26" t="s">
+      <c r="C9" s="18"/>
+      <c r="D9" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="18">
         <v>3</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="18">
         <v>10</v>
       </c>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="58" t="s">
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="N9" s="59"/>
-      <c r="O9" s="60"/>
-      <c r="P9" s="55" t="s">
+      <c r="N9" s="85"/>
+      <c r="O9" s="86"/>
+      <c r="P9" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="Q9" s="56"/>
-      <c r="R9" s="56"/>
-      <c r="S9" s="57"/>
-      <c r="T9" s="25"/>
-      <c r="U9" s="25"/>
+      <c r="Q9" s="82"/>
+      <c r="R9" s="82"/>
+      <c r="S9" s="83"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="18"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="U10" s="25"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
+      <c r="U10" s="18"/>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25"/>
-      <c r="T11" s="25"/>
-      <c r="U11" s="25"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="18"/>
+      <c r="T11" s="18"/>
+      <c r="U11" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="U4:U5"/>
+    <mergeCell ref="T4:T5"/>
+    <mergeCell ref="M4:O5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="P9:S9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="P8:S8"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="P7:S7"/>
+    <mergeCell ref="M7:O7"/>
     <mergeCell ref="B4:C5"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="P4:S4"/>
@@ -2091,30 +2312,20 @@
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="M6:O6"/>
-    <mergeCell ref="U4:U5"/>
-    <mergeCell ref="T4:T5"/>
-    <mergeCell ref="M4:O5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="P9:S9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="P8:S8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="P7:S7"/>
-    <mergeCell ref="M7:O7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="P9" r:id="rId1"/>
+    <hyperlink ref="P9" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B1:Q27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2123,43 +2334,44 @@
     <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
     <col min="6" max="6" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I1" s="81" t="s">
+      <c r="I1" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="81"/>
+      <c r="J1" s="92"/>
     </row>
     <row r="2" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="73" t="s">
+      <c r="D2" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="75"/>
-      <c r="I2" s="73" t="s">
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="95"/>
+      <c r="I2" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="75"/>
+      <c r="J2" s="95"/>
     </row>
     <row r="3" spans="2:17" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="77"/>
-      <c r="F3" s="78" t="s">
+      <c r="E3" s="89"/>
+      <c r="F3" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="79"/>
-      <c r="I3" s="16" t="s">
+      <c r="G3" s="91"/>
+      <c r="I3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="J3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="24" t="s">
+      <c r="K3" s="17" t="s">
         <v>12</v>
       </c>
       <c r="L3" s="1" t="s">
@@ -2179,373 +2391,581 @@
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="G4" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="28" t="s">
+      <c r="K4" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="28"/>
-      <c r="M4" s="29" t="s">
+      <c r="L4" s="21"/>
+      <c r="M4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="29" t="s">
+      <c r="N4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="O4" s="28" t="s">
+      <c r="O4" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="28">
+      <c r="P4" s="21">
         <v>3</v>
       </c>
-      <c r="Q4" s="28">
+      <c r="Q4" s="21">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="35">
-        <v>1</v>
-      </c>
-      <c r="E5" s="35">
-        <v>1</v>
-      </c>
-      <c r="F5" s="35">
+      <c r="D5" s="26">
+        <v>1</v>
+      </c>
+      <c r="E5" s="26">
+        <v>1</v>
+      </c>
+      <c r="F5" s="26">
         <v>0.33329999999999999</v>
       </c>
-      <c r="G5" s="35">
+      <c r="G5" s="26">
         <v>0.33329999999999999</v>
       </c>
-      <c r="I5" s="20">
-        <v>1</v>
-      </c>
-      <c r="J5" s="21">
+      <c r="I5" s="13">
+        <v>1</v>
+      </c>
+      <c r="J5" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="35">
-        <v>1</v>
-      </c>
-      <c r="E6" s="35">
-        <v>1</v>
-      </c>
-      <c r="F6" s="35">
-        <v>1</v>
-      </c>
-      <c r="G6" s="35">
-        <v>1</v>
-      </c>
-      <c r="I6" s="20">
-        <v>1</v>
-      </c>
-      <c r="J6" s="21">
+      <c r="D6" s="26">
+        <v>1</v>
+      </c>
+      <c r="E6" s="26">
+        <v>1</v>
+      </c>
+      <c r="F6" s="26">
+        <v>1</v>
+      </c>
+      <c r="G6" s="26">
+        <v>1</v>
+      </c>
+      <c r="I6" s="13">
+        <v>1</v>
+      </c>
+      <c r="J6" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="35">
-        <v>1</v>
-      </c>
-      <c r="E7" s="35">
-        <v>1</v>
-      </c>
-      <c r="F7" s="35">
+      <c r="D7" s="26">
+        <v>1</v>
+      </c>
+      <c r="E7" s="26">
+        <v>1</v>
+      </c>
+      <c r="F7" s="26">
         <v>0.33329999999999999</v>
       </c>
-      <c r="G7" s="35">
+      <c r="G7" s="26">
         <v>0.33329999999999999</v>
       </c>
-      <c r="I7" s="20">
-        <v>1</v>
-      </c>
-      <c r="J7" s="21">
+      <c r="I7" s="13">
+        <v>1</v>
+      </c>
+      <c r="J7" s="14">
         <v>0.33329999999999999</v>
       </c>
     </row>
-    <row r="8" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="35">
-        <v>1</v>
-      </c>
-      <c r="E8" s="35">
-        <v>1</v>
-      </c>
-      <c r="F8" s="35">
+      <c r="D8" s="26">
+        <v>1</v>
+      </c>
+      <c r="E8" s="26">
+        <v>1</v>
+      </c>
+      <c r="F8" s="26">
         <v>0.33329999999999999</v>
       </c>
-      <c r="G8" s="35">
+      <c r="G8" s="26">
         <v>0.33329999999999999</v>
       </c>
-      <c r="I8" s="20">
-        <v>1</v>
-      </c>
-      <c r="J8" s="21">
+      <c r="I8" s="13">
+        <v>1</v>
+      </c>
+      <c r="J8" s="14">
         <v>0.33329999999999999</v>
       </c>
     </row>
-    <row r="9" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="36">
-        <f>AVERAGE(D5:D8)</f>
-        <v>1</v>
-      </c>
-      <c r="E9" s="36">
-        <f>AVERAGE(E5:E8)</f>
-        <v>1</v>
-      </c>
-      <c r="F9" s="36">
-        <f>AVERAGE(F5:F8)</f>
-        <v>0.49997499999999995</v>
-      </c>
-      <c r="G9" s="36">
-        <f>AVERAGE(G5:G8)</f>
-        <v>0.49997499999999995</v>
-      </c>
-      <c r="I9" s="22">
-        <f>AVERAGE(I5:I8)</f>
-        <v>1</v>
-      </c>
-      <c r="J9" s="23">
-        <f>AVERAGE(J5:J8)</f>
-        <v>0.66664999999999996</v>
-      </c>
-    </row>
-    <row r="11" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="15"/>
-    </row>
-    <row r="12" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="38" t="s">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="26">
+        <v>1</v>
+      </c>
+      <c r="E9" s="26">
+        <v>1</v>
+      </c>
+      <c r="F9" s="26">
+        <v>1</v>
+      </c>
+      <c r="G9" s="26">
+        <v>1</v>
+      </c>
+      <c r="I9" s="13">
+        <v>1</v>
+      </c>
+      <c r="J9" s="14">
+        <v>0.33329999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="26">
+        <v>1</v>
+      </c>
+      <c r="E10" s="26">
+        <v>1</v>
+      </c>
+      <c r="F10" s="26">
+        <v>1</v>
+      </c>
+      <c r="G10" s="26">
+        <v>1</v>
+      </c>
+      <c r="I10" s="13">
+        <v>1</v>
+      </c>
+      <c r="J10" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B11" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="26">
+        <v>1</v>
+      </c>
+      <c r="E11" s="26">
+        <v>1</v>
+      </c>
+      <c r="F11" s="26">
+        <v>1</v>
+      </c>
+      <c r="G11" s="26">
+        <v>1</v>
+      </c>
+      <c r="I11" s="13">
+        <v>1</v>
+      </c>
+      <c r="J11" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="26">
+        <v>1</v>
+      </c>
+      <c r="E12" s="26">
+        <v>1</v>
+      </c>
+      <c r="F12" s="26">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="G12" s="26">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="I12" s="13">
+        <v>1</v>
+      </c>
+      <c r="J12" s="14">
+        <v>0.33329999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="27">
+        <f>AVERAGE(D5:D12)</f>
+        <v>1</v>
+      </c>
+      <c r="E13" s="27">
+        <f>AVERAGE(E5:E12)</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="27">
+        <f>AVERAGE(F5:F12)</f>
+        <v>0.66665000000000008</v>
+      </c>
+      <c r="G13" s="27">
+        <f>AVERAGE(G5:G12)</f>
+        <v>0.66665000000000008</v>
+      </c>
+      <c r="I13" s="15">
+        <f>AVERAGE(I5:I12)</f>
+        <v>1</v>
+      </c>
+      <c r="J13" s="16">
+        <f>AVERAGE(J5:J12)</f>
+        <v>0.66665000000000008</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="80"/>
-      <c r="I12" s="38" t="s">
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="87"/>
+      <c r="I16" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="J12" s="80"/>
-    </row>
-    <row r="13" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="76" t="s">
+      <c r="J16" s="87"/>
+    </row>
+    <row r="17" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="77"/>
-      <c r="F13" s="78" t="s">
+      <c r="E17" s="89"/>
+      <c r="F17" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="79"/>
-      <c r="I13" s="16" t="s">
+      <c r="G17" s="91"/>
+      <c r="I17" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J13" s="17" t="s">
+      <c r="J17" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B14" s="9" t="s">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C18" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D18" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="E18" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="34" t="s">
+      <c r="F18" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="34" t="s">
+      <c r="G18" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="18" t="s">
+      <c r="I18" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="J14" s="19" t="s">
+      <c r="J18" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B15" s="10" t="s">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C19" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="35">
-        <v>1</v>
-      </c>
-      <c r="E15" s="35">
-        <v>1</v>
-      </c>
-      <c r="F15" s="35">
-        <v>1</v>
-      </c>
-      <c r="G15" s="35">
-        <v>1</v>
-      </c>
-      <c r="I15" s="20">
-        <v>1</v>
-      </c>
-      <c r="J15" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B16" s="10" t="s">
+      <c r="D19" s="26">
+        <v>1</v>
+      </c>
+      <c r="E19" s="26">
+        <v>1</v>
+      </c>
+      <c r="F19" s="26">
+        <v>1</v>
+      </c>
+      <c r="G19" s="26">
+        <v>1</v>
+      </c>
+      <c r="I19" s="13">
+        <v>1</v>
+      </c>
+      <c r="J19" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B20" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C20" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="35">
-        <v>1</v>
-      </c>
-      <c r="E16" s="35">
-        <v>1</v>
-      </c>
-      <c r="F16" s="35">
+      <c r="D20" s="26">
+        <v>1</v>
+      </c>
+      <c r="E20" s="26">
+        <v>1</v>
+      </c>
+      <c r="F20" s="26">
         <v>0.71430000000000005</v>
       </c>
-      <c r="G16" s="35">
+      <c r="G20" s="26">
         <v>0.5</v>
       </c>
-      <c r="I16" s="20">
-        <v>1</v>
-      </c>
-      <c r="J16" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="10" t="s">
+      <c r="I20" s="13">
+        <v>1</v>
+      </c>
+      <c r="J20" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B21" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C21" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="35">
-        <v>1</v>
-      </c>
-      <c r="E17" s="35">
+      <c r="D21" s="26">
+        <v>1</v>
+      </c>
+      <c r="E21" s="26">
         <v>0.91669999999999996</v>
       </c>
-      <c r="F17" s="35">
+      <c r="F21" s="26">
         <v>0.72829999999999995</v>
       </c>
-      <c r="G17" s="35">
+      <c r="G21" s="26">
         <v>0.7097</v>
       </c>
-      <c r="I17" s="20">
-        <v>1</v>
-      </c>
-      <c r="J17" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="10" t="s">
+      <c r="I21" s="13">
+        <v>1</v>
+      </c>
+      <c r="J21" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C22" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="35">
+      <c r="D22" s="26">
         <v>0.3609</v>
       </c>
-      <c r="E18" s="35">
+      <c r="E22" s="26">
         <v>0.90229999999999999</v>
       </c>
-      <c r="F18" s="35">
+      <c r="F22" s="26">
         <v>0.84209999999999996</v>
       </c>
-      <c r="G18" s="35">
+      <c r="G22" s="26">
         <v>0.93020000000000003</v>
       </c>
-      <c r="I18" s="20">
-        <v>1</v>
-      </c>
-      <c r="J18" s="21">
+      <c r="I22" s="13">
+        <v>1</v>
+      </c>
+      <c r="J22" s="14">
         <v>0.70369999999999999</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D19" s="36">
-        <f>AVERAGE(D15:D18)</f>
-        <v>0.840225</v>
-      </c>
-      <c r="E19" s="36">
-        <f>AVERAGE(E15:E18)</f>
-        <v>0.95474999999999999</v>
-      </c>
-      <c r="F19" s="36">
-        <f>AVERAGE(F15:F18)</f>
-        <v>0.82117499999999999</v>
-      </c>
-      <c r="G19" s="36">
-        <f>AVERAGE(G15:G18)</f>
-        <v>0.78497499999999998</v>
-      </c>
-      <c r="I19" s="23">
-        <f>AVERAGE(I15:I18)</f>
-        <v>1</v>
-      </c>
-      <c r="J19" s="23">
-        <f>AVERAGE(J15:J18)</f>
-        <v>0.925925</v>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B23" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="26">
+        <v>1</v>
+      </c>
+      <c r="E23" s="26">
+        <v>1</v>
+      </c>
+      <c r="F23" s="26">
+        <v>1</v>
+      </c>
+      <c r="G23" s="26">
+        <v>1</v>
+      </c>
+      <c r="I23" s="13">
+        <v>1</v>
+      </c>
+      <c r="J23" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B24" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="26">
+        <v>0.4</v>
+      </c>
+      <c r="E24" s="26">
+        <v>0.8</v>
+      </c>
+      <c r="F24" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="G24" s="26">
+        <v>0.18179999999999999</v>
+      </c>
+      <c r="I24" s="13">
+        <v>1</v>
+      </c>
+      <c r="J24" s="14">
+        <v>0.27779999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B25" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="E25" s="26">
+        <v>1</v>
+      </c>
+      <c r="F25" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="26">
+        <v>0.4</v>
+      </c>
+      <c r="I25" s="13">
+        <v>1</v>
+      </c>
+      <c r="J25" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="26">
+        <v>1</v>
+      </c>
+      <c r="F26" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="G26" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="I26" s="13">
+        <v>1</v>
+      </c>
+      <c r="J26" s="14">
+        <v>4.5499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="27">
+        <f>AVERAGE(D19:D26)</f>
+        <v>0.78261250000000004</v>
+      </c>
+      <c r="E27" s="27">
+        <f t="shared" ref="E27:G27" si="0">AVERAGE(E19:E26)</f>
+        <v>0.95237499999999997</v>
+      </c>
+      <c r="F27" s="27">
+        <f t="shared" si="0"/>
+        <v>0.61558749999999995</v>
+      </c>
+      <c r="G27" s="27">
+        <f t="shared" si="0"/>
+        <v>0.59521250000000003</v>
+      </c>
+      <c r="I27" s="50">
+        <f>AVERAGE(I19:I26)</f>
+        <v>1</v>
+      </c>
+      <c r="J27" s="16">
+        <f>AVERAGE(J19:J26)</f>
+        <v>0.75337499999999991</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="I16:J16"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>

</xml_diff>

<commit_message>
update result from no-sql test
</commit_message>
<xml_diff>
--- a/hammer-colombo/nosql-examaples-set/test.xlsx
+++ b/hammer-colombo/nosql-examaples-set/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MauroRepository/My_Repository/CRISP_Progetti/Hammer_Project/git/hammer-colombo/nosql-examaples-set/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E65DC05-35C3-EB47-A1DA-3487573317ED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E19C48-53B6-AC44-8F08-CDE9BD0A6ADE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -967,6 +967,54 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -989,56 +1037,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1355,7 +1355,7 @@
   <dimension ref="B1:S12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2030,62 +2030,62 @@
       <c r="U3" s="18"/>
     </row>
     <row r="4" spans="2:21" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="61" t="s">
+      <c r="C4" s="78"/>
+      <c r="D4" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="61" t="s">
+      <c r="E4" s="79" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="69" t="s">
+      <c r="G4" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="61" t="s">
+      <c r="H4" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="80"/>
-      <c r="M4" s="74"/>
-      <c r="N4" s="75"/>
-      <c r="O4" s="76"/>
-      <c r="P4" s="62" t="s">
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+      <c r="L4" s="68"/>
+      <c r="M4" s="62"/>
+      <c r="N4" s="63"/>
+      <c r="O4" s="64"/>
+      <c r="P4" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="63"/>
-      <c r="R4" s="63"/>
-      <c r="S4" s="64"/>
-      <c r="T4" s="73"/>
-      <c r="U4" s="68"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="81"/>
+      <c r="S4" s="82"/>
+      <c r="T4" s="61"/>
+      <c r="U4" s="60"/>
     </row>
     <row r="5" spans="2:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="69"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="61"/>
-      <c r="L5" s="80"/>
-      <c r="M5" s="77"/>
-      <c r="N5" s="78"/>
-      <c r="O5" s="79"/>
-      <c r="P5" s="65" t="s">
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="86"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="66"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="66"/>
-      <c r="S5" s="67"/>
-      <c r="T5" s="73"/>
-      <c r="U5" s="68"/>
+      <c r="Q5" s="84"/>
+      <c r="R5" s="84"/>
+      <c r="S5" s="85"/>
+      <c r="T5" s="61"/>
+      <c r="U5" s="60"/>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B6" s="20" t="s">
@@ -2113,17 +2113,17 @@
       <c r="J6" s="18"/>
       <c r="K6" s="18"/>
       <c r="L6" s="18"/>
-      <c r="M6" s="70" t="s">
+      <c r="M6" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="N6" s="71"/>
-      <c r="O6" s="72"/>
-      <c r="P6" s="70">
+      <c r="N6" s="76"/>
+      <c r="O6" s="77"/>
+      <c r="P6" s="75">
         <v>3</v>
       </c>
-      <c r="Q6" s="71"/>
-      <c r="R6" s="71"/>
-      <c r="S6" s="72"/>
+      <c r="Q6" s="76"/>
+      <c r="R6" s="76"/>
+      <c r="S6" s="77"/>
       <c r="T6" s="18"/>
       <c r="U6" s="18"/>
     </row>
@@ -2147,21 +2147,21 @@
       <c r="H7" s="18">
         <v>10</v>
       </c>
-      <c r="I7" s="68"/>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
       <c r="L7" s="18"/>
-      <c r="M7" s="70" t="s">
+      <c r="M7" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="N7" s="71"/>
-      <c r="O7" s="72"/>
-      <c r="P7" s="70">
+      <c r="N7" s="76"/>
+      <c r="O7" s="77"/>
+      <c r="P7" s="75">
         <v>32</v>
       </c>
-      <c r="Q7" s="71"/>
-      <c r="R7" s="71"/>
-      <c r="S7" s="72"/>
+      <c r="Q7" s="76"/>
+      <c r="R7" s="76"/>
+      <c r="S7" s="77"/>
       <c r="T7" s="18"/>
       <c r="U7" s="18"/>
     </row>
@@ -2191,17 +2191,17 @@
       <c r="J8" s="18"/>
       <c r="K8" s="18"/>
       <c r="L8" s="18"/>
-      <c r="M8" s="70" t="s">
+      <c r="M8" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="N8" s="71"/>
-      <c r="O8" s="72"/>
-      <c r="P8" s="70">
+      <c r="N8" s="76"/>
+      <c r="O8" s="77"/>
+      <c r="P8" s="75">
         <v>3000</v>
       </c>
-      <c r="Q8" s="71"/>
-      <c r="R8" s="71"/>
-      <c r="S8" s="72"/>
+      <c r="Q8" s="76"/>
+      <c r="R8" s="76"/>
+      <c r="S8" s="77"/>
       <c r="T8" s="18"/>
       <c r="U8" s="18"/>
     </row>
@@ -2229,17 +2229,17 @@
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
       <c r="L9" s="18"/>
-      <c r="M9" s="84" t="s">
+      <c r="M9" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="N9" s="85"/>
-      <c r="O9" s="86"/>
-      <c r="P9" s="81" t="s">
+      <c r="N9" s="73"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="Q9" s="82"/>
-      <c r="R9" s="82"/>
-      <c r="S9" s="83"/>
+      <c r="Q9" s="70"/>
+      <c r="R9" s="70"/>
+      <c r="S9" s="71"/>
       <c r="T9" s="18"/>
       <c r="U9" s="18"/>
     </row>
@@ -2289,16 +2289,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="U4:U5"/>
-    <mergeCell ref="T4:T5"/>
-    <mergeCell ref="M4:O5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="P9:S9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="P8:S8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="P7:S7"/>
-    <mergeCell ref="M7:O7"/>
     <mergeCell ref="B4:C5"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="P4:S4"/>
@@ -2312,6 +2302,16 @@
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="P6:S6"/>
     <mergeCell ref="M6:O6"/>
+    <mergeCell ref="U4:U5"/>
+    <mergeCell ref="T4:T5"/>
+    <mergeCell ref="M4:O5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="P9:S9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="P8:S8"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="P7:S7"/>
+    <mergeCell ref="M7:O7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P9" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>

</xml_diff>